<commit_message>
diff major bug solved
</commit_message>
<xml_diff>
--- a/TestProject/TestProject/wwwroot/upload/Sheet1.xlsx
+++ b/TestProject/TestProject/wwwroot/upload/Sheet1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\GraduationAssesment\TestProject\TestProject\wwwroot\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE68405-3E54-4E55-A126-41DAC4549BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{37E0AD66-2AAB-4900-831D-7511500608B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" xr2:uid="{00E3A524-EC4E-456D-BA7B-A22EDF3283C9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{00E3A524-EC4E-456D-BA7B-A22EDF3283C9}"/>
   </bookViews>
   <sheets>
     <sheet name="학생성적정보" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="235">
   <si>
     <t>순번</t>
   </si>
@@ -427,18 +427,6 @@
   </si>
   <si>
     <t>Data Structure</t>
-  </si>
-  <si>
-    <t>PRI4040</t>
-  </si>
-  <si>
-    <t>기술과사회</t>
-  </si>
-  <si>
-    <t>김명진</t>
-  </si>
-  <si>
-    <t>Technology and Society</t>
   </si>
   <si>
     <t>CSE2018</t>
@@ -935,7 +923,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1022,36 +1010,6 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1367,39 +1325,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB850E5-4B36-4BA0-B5F9-6B95E4DE2680}">
-  <dimension ref="B1:W53"/>
+  <dimension ref="B1:W49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="N53" sqref="N53"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.600000000000001" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="4.5703125" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" customWidth="1"/>
+    <col min="2" max="3" width="4.69921875" customWidth="1"/>
+    <col min="4" max="4" width="6.19921875" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="9.92578125" customWidth="1"/>
-    <col min="8" max="8" width="2.640625" customWidth="1"/>
-    <col min="9" max="9" width="25.92578125" customWidth="1"/>
+    <col min="7" max="7" width="9.796875" customWidth="1"/>
+    <col min="8" max="8" width="2.69921875" customWidth="1"/>
+    <col min="9" max="9" width="25.796875" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
     <col min="11" max="11" width="4.5" customWidth="1"/>
-    <col min="12" max="12" width="4.0703125" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" customWidth="1"/>
-    <col min="14" max="14" width="8.78515625" customWidth="1"/>
+    <col min="12" max="12" width="4.19921875" customWidth="1"/>
+    <col min="13" max="13" width="9.296875" customWidth="1"/>
+    <col min="14" max="14" width="8.69921875" customWidth="1"/>
     <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="6.7109375" customWidth="1"/>
-    <col min="17" max="17" width="7.85546875" customWidth="1"/>
-    <col min="18" max="18" width="11.640625" customWidth="1"/>
-    <col min="19" max="19" width="9.92578125" customWidth="1"/>
+    <col min="16" max="16" width="6.69921875" customWidth="1"/>
+    <col min="17" max="17" width="7.796875" customWidth="1"/>
+    <col min="18" max="18" width="11.69921875" customWidth="1"/>
+    <col min="19" max="19" width="9.796875" customWidth="1"/>
     <col min="20" max="20" width="15.5" customWidth="1"/>
     <col min="21" max="21" width="22" customWidth="1"/>
-    <col min="22" max="22" width="25.92578125" customWidth="1"/>
-    <col min="23" max="23" width="8.640625" customWidth="1"/>
+    <col min="22" max="22" width="25.796875" customWidth="1"/>
+    <col min="23" max="23" width="8.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:23" ht="21.6" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1467,7 +1424,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B2" s="3">
         <v>1</v>
       </c>
@@ -1527,7 +1484,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B3" s="9">
         <v>2</v>
       </c>
@@ -1581,7 +1538,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:23" ht="21.6" x14ac:dyDescent="0.4">
       <c r="B4" s="15">
         <v>3</v>
       </c>
@@ -1635,7 +1592,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B5" s="9">
         <v>4</v>
       </c>
@@ -1691,7 +1648,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B6" s="15">
         <v>5</v>
       </c>
@@ -1747,7 +1704,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B7" s="9">
         <v>6</v>
       </c>
@@ -1801,7 +1758,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:23" ht="21.6" x14ac:dyDescent="0.4">
       <c r="B8" s="15">
         <v>7</v>
       </c>
@@ -1855,7 +1812,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B9" s="9">
         <v>8</v>
       </c>
@@ -1915,7 +1872,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:23" ht="21.6" x14ac:dyDescent="0.4">
       <c r="B10" s="15">
         <v>9</v>
       </c>
@@ -1952,10 +1909,10 @@
         <v>30</v>
       </c>
       <c r="Q10" s="15" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="R10" s="15" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="S10" s="15"/>
       <c r="T10" s="20"/>
@@ -1969,7 +1926,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:23" ht="21.6" x14ac:dyDescent="0.4">
       <c r="B11" s="9">
         <v>10</v>
       </c>
@@ -2023,7 +1980,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B12" s="15">
         <v>11</v>
       </c>
@@ -2077,7 +2034,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:23" ht="21.6" x14ac:dyDescent="0.4">
       <c r="B13" s="9">
         <v>12</v>
       </c>
@@ -2133,7 +2090,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:23" ht="21.6" x14ac:dyDescent="0.4">
       <c r="B14" s="15">
         <v>13</v>
       </c>
@@ -2191,7 +2148,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B15" s="9">
         <v>14</v>
       </c>
@@ -2245,7 +2202,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B16" s="15">
         <v>15</v>
       </c>
@@ -2299,7 +2256,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B17" s="9">
         <v>16</v>
       </c>
@@ -2353,7 +2310,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B18" s="15">
         <v>17</v>
       </c>
@@ -2407,7 +2364,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B19" s="9">
         <v>18</v>
       </c>
@@ -2461,7 +2418,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B20" s="15">
         <v>19</v>
       </c>
@@ -2517,7 +2474,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B21" s="9">
         <v>20</v>
       </c>
@@ -2571,7 +2528,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B22" s="15">
         <v>21</v>
       </c>
@@ -2627,1208 +2584,1103 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="B23" s="9">
+    <row r="23" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B23" s="15">
+        <v>23</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="K23" s="19">
+        <v>3</v>
+      </c>
+      <c r="L23" s="17"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="P23" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q23" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="R23" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="S23" s="15"/>
+      <c r="T23" s="20"/>
+      <c r="U23" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="V23" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="W23" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B24" s="9">
+        <v>24</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="K24" s="13">
+        <v>3</v>
+      </c>
+      <c r="L24" s="11"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="P24" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q24" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="R24" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="S24" s="9"/>
+      <c r="T24" s="14"/>
+      <c r="U24" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="V24" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="W24" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:23" ht="21.6" x14ac:dyDescent="0.4">
+      <c r="B25" s="15">
+        <v>25</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="I25" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="K25" s="19">
+        <v>3</v>
+      </c>
+      <c r="L25" s="17"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="P25" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q25" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="R25" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="S25" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="T25" s="20"/>
+      <c r="U25" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="V25" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="W25" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B26" s="9">
+        <v>26</v>
+      </c>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="K26" s="13">
+        <v>2</v>
+      </c>
+      <c r="L26" s="11"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="P26" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q26" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="R26" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="S26" s="9"/>
+      <c r="T26" s="14"/>
+      <c r="U26" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="V26" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="W26" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" ht="21.6" x14ac:dyDescent="0.4">
+      <c r="B27" s="15">
+        <v>27</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I27" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="J27" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="K27" s="19">
+        <v>4</v>
+      </c>
+      <c r="L27" s="17"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="P27" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q27" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="R27" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="S27" s="15"/>
+      <c r="T27" s="20"/>
+      <c r="U27" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="V27" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="W27" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B28" s="9">
+        <v>28</v>
+      </c>
+      <c r="C28" s="10"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="K28" s="13">
+        <v>3</v>
+      </c>
+      <c r="L28" s="11"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="P28" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q28" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="R28" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="S28" s="9"/>
+      <c r="T28" s="14"/>
+      <c r="U28" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="V28" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="W28" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B29" s="15">
+        <v>29</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11" t="s">
+      <c r="E29" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F29" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G23" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="H23" s="11" t="s">
+      <c r="G29" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="J29" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="K29" s="19">
+        <v>3</v>
+      </c>
+      <c r="L29" s="17"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="P29" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q29" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="R29" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="S29" s="15"/>
+      <c r="T29" s="20"/>
+      <c r="U29" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="V29" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="W29" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="2:23" ht="21.6" x14ac:dyDescent="0.4">
+      <c r="B30" s="9">
+        <v>30</v>
+      </c>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="K30" s="13">
+        <v>4</v>
+      </c>
+      <c r="L30" s="11"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="P30" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q30" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="R30" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="S30" s="9"/>
+      <c r="T30" s="14"/>
+      <c r="U30" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="V30" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="W30" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B31" s="15">
+        <v>31</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="H31" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I31" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="J31" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="K31" s="19">
+        <v>3</v>
+      </c>
+      <c r="L31" s="17"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="P31" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q31" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="R31" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="S31" s="15"/>
+      <c r="T31" s="20"/>
+      <c r="U31" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="V31" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="W31" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B32" s="9">
+        <v>32</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="J32" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="K32" s="13">
+        <v>1</v>
+      </c>
+      <c r="L32" s="11"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="P32" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q32" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="R32" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="S32" s="9"/>
+      <c r="T32" s="14"/>
+      <c r="U32" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="V32" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="W32" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B33" s="15">
+        <v>33</v>
+      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="H33" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="I23" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="J23" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="K23" s="13">
-        <v>3</v>
-      </c>
-      <c r="L23" s="11"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="P23" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q23" s="11" t="s">
+      <c r="I33" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="J33" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="K33" s="19">
+        <v>3</v>
+      </c>
+      <c r="L33" s="17"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="P33" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q33" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="R33" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="S33" s="15"/>
+      <c r="T33" s="20"/>
+      <c r="U33" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="V33" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="W33" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B34" s="9">
+        <v>34</v>
+      </c>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="K34" s="13">
+        <v>1</v>
+      </c>
+      <c r="L34" s="11"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="P34" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q34" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="R23" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="S23" s="9"/>
-      <c r="T23" s="14"/>
-      <c r="U23" s="11" t="s">
+      <c r="R34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="S34" s="9"/>
+      <c r="T34" s="14"/>
+      <c r="U34" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="V23" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="W23" s="11" t="s">
+      <c r="V34" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="W34" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="B24" s="15">
-        <v>23</v>
-      </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="H24" s="17" t="s">
+    <row r="35" spans="2:23" ht="21.6" x14ac:dyDescent="0.4">
+      <c r="B35" s="15">
         <v>35</v>
       </c>
-      <c r="I24" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="J24" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="K24" s="19">
-        <v>3</v>
-      </c>
-      <c r="L24" s="17"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="P24" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q24" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="R24" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="S24" s="15"/>
-      <c r="T24" s="20"/>
-      <c r="U24" s="17" t="s">
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="I35" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="J35" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="K35" s="19">
+        <v>3</v>
+      </c>
+      <c r="L35" s="17"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="P35" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q35" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="R35" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="S35" s="15"/>
+      <c r="T35" s="20"/>
+      <c r="U35" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="V24" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="W24" s="17" t="s">
+      <c r="V35" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="W35" s="17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="B25" s="9">
-        <v>24</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="I25" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="J25" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="K25" s="13">
-        <v>3</v>
-      </c>
-      <c r="L25" s="11"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="P25" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q25" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="R25" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="S25" s="9"/>
-      <c r="T25" s="14"/>
-      <c r="U25" s="11" t="s">
+    <row r="36" spans="2:23" ht="21.6" x14ac:dyDescent="0.4">
+      <c r="B36" s="9">
+        <v>36</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="K36" s="13">
+        <v>3</v>
+      </c>
+      <c r="L36" s="11"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="P36" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q36" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="R36" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="S36" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="T36" s="14"/>
+      <c r="U36" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="V25" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="W25" s="11" t="s">
+      <c r="V36" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="W36" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
-      <c r="B26" s="15">
-        <v>25</v>
-      </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G26" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="H26" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="I26" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="J26" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="K26" s="19">
-        <v>3</v>
-      </c>
-      <c r="L26" s="17"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="P26" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q26" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="R26" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="S26" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="T26" s="20"/>
-      <c r="U26" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="V26" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="W26" s="17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="B27" s="9">
-        <v>26</v>
-      </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="I27" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="J27" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="K27" s="13">
-        <v>2</v>
-      </c>
-      <c r="L27" s="11"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="P27" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q27" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="R27" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="S27" s="9"/>
-      <c r="T27" s="14"/>
-      <c r="U27" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="V27" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="W27" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
-      <c r="B28" s="15">
-        <v>27</v>
-      </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F28" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="G28" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="H28" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="I28" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="J28" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="K28" s="19">
-        <v>4</v>
-      </c>
-      <c r="L28" s="17"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="P28" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q28" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="R28" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="S28" s="15"/>
-      <c r="T28" s="20"/>
-      <c r="U28" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="V28" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="W28" s="17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="B29" s="9">
-        <v>28</v>
-      </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="I29" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="J29" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="K29" s="13">
-        <v>3</v>
-      </c>
-      <c r="L29" s="11"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="P29" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q29" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="R29" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="S29" s="9"/>
-      <c r="T29" s="14"/>
-      <c r="U29" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="V29" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="W29" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="B30" s="15">
-        <v>29</v>
-      </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F30" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="H30" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="I30" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="J30" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="K30" s="19">
-        <v>3</v>
-      </c>
-      <c r="L30" s="17"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="P30" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q30" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="R30" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="S30" s="15"/>
-      <c r="T30" s="20"/>
-      <c r="U30" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="V30" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="W30" s="17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
-      <c r="B31" s="9">
-        <v>30</v>
-      </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="H31" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="I31" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="J31" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="K31" s="13">
-        <v>4</v>
-      </c>
-      <c r="L31" s="11"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="P31" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q31" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="R31" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="S31" s="9"/>
-      <c r="T31" s="14"/>
-      <c r="U31" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="V31" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="W31" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="B32" s="15">
-        <v>31</v>
-      </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F32" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="G32" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="H32" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="I32" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="J32" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="K32" s="19">
-        <v>3</v>
-      </c>
-      <c r="L32" s="17"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="P32" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q32" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="R32" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="S32" s="15"/>
-      <c r="T32" s="20"/>
-      <c r="U32" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="V32" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="W32" s="17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="B33" s="9">
-        <v>32</v>
-      </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="H33" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="I33" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="J33" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="K33" s="13">
+    <row r="37" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="C37">
+        <v>2021</v>
+      </c>
+      <c r="D37" t="s">
+        <v>192</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="F37" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="I37" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="J37" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="K37" s="24">
+        <v>3</v>
+      </c>
+      <c r="P37" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q37" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="R37" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="S37" s="25" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="38" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="E38" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="G38" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="I38" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="J38" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="K38" s="27">
+        <v>3</v>
+      </c>
+      <c r="P38" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q38" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="R38" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="S38" s="28" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="E39" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="G39" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="I39" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="J39" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="K39" s="24">
+        <v>3</v>
+      </c>
+      <c r="P39" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q39" s="22" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="E40" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="G40" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="I40" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="J40" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="K40" s="27">
+        <v>3</v>
+      </c>
+      <c r="P40" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q40" s="21" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="E41" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="G41" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="I41" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="J41" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="K41" s="24">
+        <v>3</v>
+      </c>
+      <c r="P41" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q41" s="22" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="E42" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="G42" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="I42" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="J42" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="K42" s="27">
+        <v>3</v>
+      </c>
+      <c r="P42" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q42" s="21" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="43" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="E43" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="F43" t="s">
+        <v>194</v>
+      </c>
+      <c r="G43" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="I43" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="J43" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="K43" s="24">
         <v>1</v>
       </c>
-      <c r="L33" s="11"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="P33" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q33" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="R33" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="S33" s="9"/>
-      <c r="T33" s="14"/>
-      <c r="U33" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="V33" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="W33" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="B34" s="15">
-        <v>33</v>
-      </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F34" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="H34" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="I34" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="J34" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K34" s="19">
-        <v>3</v>
-      </c>
-      <c r="L34" s="17"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="P34" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q34" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="R34" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="S34" s="15"/>
-      <c r="T34" s="20"/>
-      <c r="U34" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="V34" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="W34" s="17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="B35" s="9">
-        <v>34</v>
-      </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="I35" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="J35" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="K35" s="13">
-        <v>1</v>
-      </c>
-      <c r="L35" s="11"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="P35" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q35" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="R35" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="S35" s="9"/>
-      <c r="T35" s="14"/>
-      <c r="U35" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="V35" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="W35" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
-      <c r="B36" s="15">
-        <v>35</v>
-      </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="F36" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="G36" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="H36" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="I36" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="J36" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="K36" s="19">
-        <v>3</v>
-      </c>
-      <c r="L36" s="17"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="P36" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q36" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="R36" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="S36" s="15"/>
-      <c r="T36" s="20"/>
-      <c r="U36" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="V36" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="W36" s="17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
-      <c r="B37" s="9">
-        <v>36</v>
-      </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="H37" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="I37" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="J37" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="K37" s="13">
-        <v>3</v>
-      </c>
-      <c r="L37" s="11"/>
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
-      <c r="O37" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="P37" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q37" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="R37" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="S37" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="T37" s="14"/>
-      <c r="U37" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="V37" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="W37" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="C38">
-        <v>2021</v>
-      </c>
-      <c r="D38" t="s">
-        <v>196</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="F38" s="23" t="s">
+      <c r="P43" s="22" t="s">
         <v>198</v>
       </c>
-      <c r="G38" s="22" t="s">
+      <c r="Q43" s="22" t="s">
         <v>199</v>
       </c>
-      <c r="I38" s="23" t="s">
-        <v>200</v>
-      </c>
-      <c r="J38" s="22" t="s">
+    </row>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="E44" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="G44" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="I44" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="J44" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="K44" s="27">
+        <v>3</v>
+      </c>
+      <c r="P44" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q44" s="21" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="45" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="C45">
+        <v>2022</v>
+      </c>
+      <c r="D45" t="s">
+        <v>218</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="G45" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="I45" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="J45" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="K45" s="24">
+        <v>3</v>
+      </c>
+      <c r="P45" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q45" s="22" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="E46" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="G46" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="I46" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="J46" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="K46" s="27">
+        <v>3</v>
+      </c>
+      <c r="P46" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q46" s="21" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="47" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="E47" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="G47" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="I47" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="J47" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="K47" s="24">
+        <v>3</v>
+      </c>
+      <c r="P47" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q47" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="S47" t="s">
         <v>201</v>
       </c>
-      <c r="K38" s="24">
-        <v>3</v>
-      </c>
-      <c r="P38" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q38" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="R38" s="22" t="s">
-        <v>204</v>
-      </c>
-      <c r="S38" s="25" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="E39" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="G39" s="21" t="s">
-        <v>206</v>
-      </c>
-      <c r="I39" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="J39" s="21" t="s">
+    </row>
+    <row r="48" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="E48" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="G48" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="I48" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="J48" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="K48" s="27">
+        <v>3</v>
+      </c>
+      <c r="P48" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q48" s="21" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="49" spans="5:17" x14ac:dyDescent="0.4">
+      <c r="E49" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="G49" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="I49" s="23" t="s">
+        <v>229</v>
+      </c>
+      <c r="J49" s="22" t="s">
         <v>208</v>
       </c>
-      <c r="K39" s="27">
-        <v>3</v>
-      </c>
-      <c r="P39" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="Q39" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="R39" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="S39" s="28" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="E40" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="G40" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="I40" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="J40" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="K40" s="24">
-        <v>3</v>
-      </c>
-      <c r="P40" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q40" s="22" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="E41" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="G41" s="21" t="s">
-        <v>213</v>
-      </c>
-      <c r="I41" s="26" t="s">
-        <v>214</v>
-      </c>
-      <c r="J41" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="K41" s="27">
-        <v>3</v>
-      </c>
-      <c r="P41" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q41" s="21" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="E42" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="G42" s="22" t="s">
-        <v>219</v>
-      </c>
-      <c r="I42" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="J42" s="22" t="s">
-        <v>217</v>
-      </c>
-      <c r="K42" s="24">
-        <v>3</v>
-      </c>
-      <c r="P42" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q42" s="22" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="E43" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="G43" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="I43" s="26" t="s">
-        <v>220</v>
-      </c>
-      <c r="J43" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="K43" s="27">
-        <v>3</v>
-      </c>
-      <c r="P43" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q43" s="21" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="E44" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="K49" s="24">
+        <v>3</v>
+      </c>
+      <c r="P49" s="22" t="s">
         <v>198</v>
       </c>
-      <c r="G44" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="I44" s="23" t="s">
-        <v>235</v>
-      </c>
-      <c r="J44" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="K44" s="24">
-        <v>1</v>
-      </c>
-      <c r="P44" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q44" s="22" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="E45" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="G45" s="21" t="s">
-        <v>236</v>
-      </c>
-      <c r="I45" s="26" t="s">
-        <v>237</v>
-      </c>
-      <c r="J45" s="21" t="s">
-        <v>238</v>
-      </c>
-      <c r="K45" s="27">
-        <v>3</v>
-      </c>
-      <c r="P45" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q45" s="21" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="C46">
-        <v>2022</v>
-      </c>
-      <c r="D46" t="s">
-        <v>222</v>
-      </c>
-      <c r="E46" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="G46" s="22" t="s">
-        <v>223</v>
-      </c>
-      <c r="I46" s="23" t="s">
-        <v>224</v>
-      </c>
-      <c r="J46" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="K46" s="24">
-        <v>3</v>
-      </c>
-      <c r="P46" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q46" s="22" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="E47" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="G47" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="I47" s="26" t="s">
-        <v>226</v>
-      </c>
-      <c r="J47" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="K47" s="27">
-        <v>3</v>
-      </c>
-      <c r="P47" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q47" s="21" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="48" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="E48" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="G48" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="I48" s="23" t="s">
-        <v>229</v>
-      </c>
-      <c r="J48" s="22" t="s">
-        <v>221</v>
-      </c>
-      <c r="K48" s="24">
-        <v>3</v>
-      </c>
-      <c r="P48" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q48" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="S48" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="E49" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="G49" s="21" t="s">
-        <v>230</v>
-      </c>
-      <c r="I49" s="26" t="s">
-        <v>231</v>
-      </c>
-      <c r="J49" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="K49" s="27">
-        <v>3</v>
-      </c>
-      <c r="P49" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q49" s="21" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="50" spans="2:23" ht="18.45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="E50" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="G50" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="I50" s="23" t="s">
-        <v>233</v>
-      </c>
-      <c r="J50" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="K50" s="24">
-        <v>3</v>
-      </c>
-      <c r="P50" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q50" s="22" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="51" spans="2:23" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B51" s="30"/>
-      <c r="C51" s="30"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="25"/>
-      <c r="F51" s="31"/>
-      <c r="G51" s="25"/>
-      <c r="H51" s="25"/>
-      <c r="I51" s="31"/>
-      <c r="J51" s="25"/>
-      <c r="K51" s="32"/>
-      <c r="L51" s="25"/>
-      <c r="M51" s="30"/>
-      <c r="N51" s="30"/>
-      <c r="O51" s="25"/>
-      <c r="P51" s="25"/>
-      <c r="Q51" s="25"/>
-      <c r="R51" s="25"/>
-      <c r="S51" s="30"/>
-      <c r="T51" s="33"/>
-      <c r="U51" s="25"/>
-      <c r="V51" s="31"/>
-      <c r="W51" s="25"/>
-    </row>
-    <row r="52" spans="2:23" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B52" s="35"/>
-      <c r="C52" s="35"/>
-      <c r="D52" s="35"/>
-      <c r="E52" s="28"/>
-      <c r="F52" s="36"/>
-      <c r="G52" s="28"/>
-      <c r="H52" s="28"/>
-      <c r="I52" s="36"/>
-      <c r="J52" s="28"/>
-      <c r="K52" s="37"/>
-      <c r="L52" s="28"/>
-      <c r="M52" s="35"/>
-      <c r="N52" s="35"/>
-      <c r="O52" s="28"/>
-      <c r="P52" s="28"/>
-      <c r="Q52" s="28"/>
-      <c r="R52" s="28"/>
-      <c r="S52" s="35"/>
-      <c r="T52" s="38"/>
-      <c r="U52" s="28"/>
-      <c r="V52" s="36"/>
-      <c r="W52" s="28"/>
-    </row>
-    <row r="53" spans="2:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="J53" s="29"/>
+      <c r="Q49" s="22" t="s">
+        <v>199</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>